<commit_message>
Opraveny chyby v prednasce P7 pro anglicany
</commit_message>
<xml_diff>
--- a/PrednaskyEN/P7/frekvChar2.xlsx
+++ b/PrednaskyEN/P7/frekvChar2.xlsx
@@ -16,9 +16,6 @@
     <sheet name="List2" sheetId="3" r:id="rId2"/>
     <sheet name="List3" sheetId="4" r:id="rId3"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId4"/>
-  </externalReferences>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1027,7 +1024,7 @@
           <c:idx val="4"/>
           <c:order val="3"/>
           <c:tx>
-            <c:v>Cs = 15 pF</c:v>
+            <c:v>Cp = 15 pF</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -1082,11 +1079,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="438713328"/>
-        <c:axId val="438712768"/>
+        <c:axId val="127051840"/>
+        <c:axId val="127052400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="438713328"/>
+        <c:axId val="127051840"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1207,12 +1204,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="438712768"/>
+        <c:crossAx val="127052400"/>
         <c:crossesAt val="1.0000000000000002E-2"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="438712768"/>
+        <c:axId val="127052400"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1333,7 +1330,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="438713328"/>
+        <c:crossAx val="127051840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1731,11 +1728,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="434799216"/>
-        <c:axId val="434799776"/>
+        <c:axId val="127055200"/>
+        <c:axId val="127055760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="434799216"/>
+        <c:axId val="127055200"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1856,12 +1853,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="434799776"/>
+        <c:crossAx val="127055760"/>
         <c:crossesAt val="1.0000000000000002E-2"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="434799776"/>
+        <c:axId val="127055760"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1982,7 +1979,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="434799216"/>
+        <c:crossAx val="127055200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2343,11 +2340,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="407162096"/>
-        <c:axId val="407159856"/>
+        <c:axId val="127058000"/>
+        <c:axId val="127058560"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="407162096"/>
+        <c:axId val="127058000"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2468,12 +2465,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="407159856"/>
+        <c:crossAx val="127058560"/>
         <c:crossesAt val="-100"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="407159856"/>
+        <c:axId val="127058560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -2615,7 +2612,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="407162096"/>
+        <c:crossAx val="127058000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4433,441 +4430,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="List1"/>
-      <sheetName val="List2"/>
-      <sheetName val="List3"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="2">
-          <cell r="A2">
-            <v>1000</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3">
-            <v>1122.0184543019636</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4">
-            <v>1258.9254117941668</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5">
-            <v>1412.5375446227531</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6">
-            <v>1584.8931924611115</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7">
-            <v>1778.2794100389197</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8">
-            <v>1995.262314968877</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9">
-            <v>2238.7211385683354</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10">
-            <v>2511.8864315095743</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11">
-            <v>2818.3829312644461</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12">
-            <v>3162.277660168369</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="A13">
-            <v>3548.1338923357416</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="A14">
-            <v>3981.071705534956</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="A15">
-            <v>4466.8359215096107</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="A16">
-            <v>5011.8723362726969</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="A17">
-            <v>5623.4132519034592</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="A18">
-            <v>6309.5734448018939</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="A19">
-            <v>7079.4578438413328</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="A20">
-            <v>7943.282347242759</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="A21">
-            <v>8912.5093813373878</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="A22">
-            <v>9999.99999999992</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="A23">
-            <v>11220.184543019539</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="A24">
-            <v>12589.254117941558</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="A25">
-            <v>14125.375446227436</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="A26">
-            <v>15848.931924611006</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="A27">
-            <v>17782.794100389074</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="A28">
-            <v>19952.623149688614</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="A29">
-            <v>22387.211385683182</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="A30">
-            <v>25118.864315095547</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="A31">
-            <v>28183.82931264424</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="A32">
-            <v>31622.776601683447</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="A33">
-            <v>35481.338923357136</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="A34">
-            <v>39810.717055349247</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="A35">
-            <v>44668.359215095756</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="A36">
-            <v>50118.723362726581</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="A37">
-            <v>56234.132519034152</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="A38">
-            <v>63095.734448018447</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="A39">
-            <v>70794.578438412776</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="A40">
-            <v>79432.823472426971</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="A41">
-            <v>89125.093813373183</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="A42">
-            <v>100000</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1">
-        <row r="2">
-          <cell r="O2">
-            <v>-89.963857319189486</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="O3">
-            <v>-89.959405586613229</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="O4">
-            <v>-89.954393338080038</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="O5">
-            <v>-89.948744926776598</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="O6">
-            <v>-89.94237239846224</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="O7">
-            <v>-89.935172652816419</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="O8">
-            <v>-89.927023652436901</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="O9">
-            <v>-89.917779268451014</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="O10">
-            <v>-89.907262141804267</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="O11">
-            <v>-89.895253603945051</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="O12">
-            <v>-89.881479151041034</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="O13">
-            <v>-89.865587038515883</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="O14">
-            <v>-89.847115944777826</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="O15">
-            <v>-89.825444720036145</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="O16">
-            <v>-89.799711679093534</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="O17">
-            <v>-89.768679813334742</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="O18">
-            <v>-89.730500810696512</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="O19">
-            <v>-89.682277257434464</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="O20">
-            <v>-89.619189109183694</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="O21">
-            <v>-89.532579090216245</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="O22">
-            <v>-89.405192242243302</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="O23">
-            <v>-89.197011383522394</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="O24">
-            <v>-88.789381494407181</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="O25">
-            <v>-87.606157419902274</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="O26">
-            <v>-39.969875032937409</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="O27">
-            <v>87.42469738250665</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="O28">
-            <v>88.743704036164232</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="O29">
-            <v>89.176499473888981</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="O30">
-            <v>89.393498317028062</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="O31">
-            <v>89.5249763215798</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="O32">
-            <v>89.613818240316476</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="O33">
-            <v>89.67826134804487</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="O34">
-            <v>89.727372987000265</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="O35">
-            <v>89.766168866316363</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="O36">
-            <v>89.797649252693446</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="O37">
-            <v>89.823720646342181</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="O38">
-            <v>89.845654934058373</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="O39">
-            <v>89.864335709781102</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="O40">
-            <v>89.880398432977429</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="O41">
-            <v>89.894314088893964</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="O42">
-            <v>89.906441142217929</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2">
-        <row r="60">
-          <cell r="D60" t="str">
-            <v>C = 10 nF</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv Office">
   <a:themeElements>
@@ -8057,8 +7619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I42" sqref="I42"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V32" sqref="V32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>